<commit_message>
updtaed data with more details todied up tables added links
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F7A57F1-302A-499A-BCDB-56948C242903}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A3773B6-8630-4AC0-B2C2-301527A7B418}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Data​</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Employment rate​</t>
   </si>
   <si>
-    <t>​</t>
-  </si>
-  <si>
     <t>Download data​</t>
   </si>
   <si>
@@ -68,22 +65,43 @@
     <t>FE and skills learner achievement​</t>
   </si>
   <si>
-    <t>&lt;Direct link to datatable&gt;​</t>
-  </si>
-  <si>
-    <t>2021-22 provisional to Jul 2022 (8 Jul 2022)​</t>
-  </si>
-  <si>
-    <t>2021-22 (Nov 22)​</t>
-  </si>
-  <si>
     <t>Latest period (release date)​</t>
   </si>
   <si>
     <t>FE and skills learner achievements by SSA tier 1​</t>
   </si>
   <si>
-    <t>Annual Population Survey</t>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;Annual Population Survey&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Jul 2021 - Jun 2022 (11/10/22)</t>
+  </si>
+  <si>
+    <t>Oct 2021 - Sep 2022 (17/01/23)</t>
+  </si>
+  <si>
+    <t>January 2017 to January 2022 (25/05/22)</t>
+  </si>
+  <si>
+    <t>To be announced</t>
+  </si>
+  <si>
+    <t>2021-22 full year (Nov 22)​</t>
+  </si>
+  <si>
+    <t>2021-22 provisional to Apr 2022 (20/07/22)​</t>
+  </si>
+  <si>
+    <t>2020-21 full year (25/11/21)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS: job adverts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/3960ad0f-fd8a-49bb-91d7-f3ca1181b93f'&gt;DfE: ILR&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;DfE: ILR&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -99,29 +117,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="7"/>
+      <color rgb="FF232629"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -129,35 +139,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,7 +463,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -507,92 +497,88 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{E9E366FD-2A30-4584-A08B-C139A95416A8}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D9175CB7-D227-4323-8D32-134B39708049}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data links to table
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A3773B6-8630-4AC0-B2C2-301527A7B418}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE2403D8-5D17-4669-AE1E-009B7F3162F5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Data​</t>
   </si>
@@ -47,13 +47,7 @@
     <t>Next period (release date)​</t>
   </si>
   <si>
-    <t>Dashboard data​</t>
-  </si>
-  <si>
     <t>Employment rate​</t>
-  </si>
-  <si>
-    <t>Download data​</t>
   </si>
   <si>
     <t>Employment percentage by occupation (sub-major SOC group)​</t>
@@ -460,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,10 +466,9 @@
     <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,98 +476,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the data table text corrected some downloads shifted the tabs order
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE2403D8-5D17-4669-AE1E-009B7F3162F5}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F615A86-616E-47CF-8EA8-08018BFDB9A9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -47,24 +47,9 @@
     <t>Next period (release date)​</t>
   </si>
   <si>
-    <t>Employment rate​</t>
-  </si>
-  <si>
-    <t>Employment percentage by occupation (sub-major SOC group)​</t>
-  </si>
-  <si>
-    <t>Online job vacancy​</t>
-  </si>
-  <si>
-    <t>FE and skills learner achievement​</t>
-  </si>
-  <si>
     <t>Latest period (release date)​</t>
   </si>
   <si>
-    <t>FE and skills learner achievements by SSA tier 1​</t>
-  </si>
-  <si>
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;Annual Population Survey&lt;/a&gt;</t>
   </si>
   <si>
@@ -74,35 +59,50 @@
     <t>Oct 2021 - Sep 2022 (17/01/23)</t>
   </si>
   <si>
-    <t>January 2017 to January 2022 (25/05/22)</t>
-  </si>
-  <si>
     <t>To be announced</t>
   </si>
   <si>
-    <t>2021-22 full year (Nov 22)​</t>
-  </si>
-  <si>
-    <t>2021-22 provisional to Apr 2022 (20/07/22)​</t>
-  </si>
-  <si>
-    <t>2020-21 full year (25/11/21)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS: job adverts&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/3960ad0f-fd8a-49bb-91d7-f3ca1181b93f'&gt;DfE: ILR&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;DfE: ILR&lt;/a&gt;</t>
+    <t>Employment rates</t>
+  </si>
+  <si>
+    <t>Employment share by occupation</t>
+  </si>
+  <si>
+    <t>Online job adverts by local authority</t>
+  </si>
+  <si>
+    <t>Further education and skills achievements</t>
+  </si>
+  <si>
+    <t>Further education and skills achievements by sector subject area</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS online job adverts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/3960ad0f-fd8a-49bb-91d7-f3ca1181b93f'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Jan 2022 (25/05/22)</t>
+  </si>
+  <si>
+    <t>Aug 2020 – Jul 2021 (25/11/21)</t>
+  </si>
+  <si>
+    <t>Aug 2021 – Apr 2022 (provisional) (20/07/22)</t>
+  </si>
+  <si>
+    <t>Aug 2021 – Jul 2022 (Nov 22)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +115,13 @@
       <color rgb="FF232629"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,9 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +467,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,80 +486,80 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected some text added a note on the ONS problem corrected a data
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F615A86-616E-47CF-8EA8-08018BFDB9A9}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C25080C-34D2-4A20-8BE1-18EDB4339086}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Data​</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +517,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Updated - new data
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F615A86-616E-47CF-8EA8-08018BFDB9A9}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4194F46-B515-4799-837E-1DBB979B4250}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Data​</t>
   </si>
@@ -96,6 +96,39 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Enterprise by employment size</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Count&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Oct 2021 - Sept 2022 (28/09/22)</t>
+  </si>
+  <si>
+    <t>Oct 2022 - Sept 2023 (03/10/23)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/c9f44a09-4239-40d6-8f07-87c2b97fc5fc'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2019 -  Jul 2020 (2019 leavers) (21/10/21)</t>
+  </si>
+  <si>
+    <t>Aug 2020 - Jul 2021 (2020 leavers) (20/10/22)</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/6ed2058c-1ff4-4e13-b167-3b15bb6a0675'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2019 - Jul 2020 (2019 leavers) (09/12/21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Stage 5 (KS5) destinations </t>
   </si>
 </sst>
 </file>
@@ -111,14 +144,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF232629"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,10 +180,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,10 +527,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
@@ -507,10 +541,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
@@ -521,10 +555,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
@@ -535,31 +569,73 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data soureces table
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C25080C-34D2-4A20-8BE1-18EDB4339086}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F91C816-E7E6-4451-8E01-9FE0C50046F0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Data​</t>
   </si>
@@ -98,7 +98,37 @@
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Jan 2021 - Dec 2021 (12/04/22)</t>
+    <t>Enterprise by employment size</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Count&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Oct 2021 - Sept 2022 (28/09/22)</t>
+  </si>
+  <si>
+    <t>Oct 2022 - Sept 2023 (03/10/23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/c9f44a09-4239-40d6-8f07-87c2b97fc5fc'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2019 -  Jul 2020 (2019 leavers) (21/10/21)</t>
+  </si>
+  <si>
+    <t>Aug 2020 - Jul 2021 (2020 leavers) (20/10/22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Stage 5 (KS5) destinations </t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/6ed2058c-1ff4-4e13-b167-3b15bb6a0675'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2019 - Jul 2020 (2019 leavers) (09/12/21)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,7 +508,7 @@
     <col min="1" max="1" width="53.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
@@ -517,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -563,6 +593,48 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data sources table
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F91C816-E7E6-4451-8E01-9FE0C50046F0}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C28A7411-5C3D-4DD3-9954-5D31439669D8}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,14 +144,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF232629"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color rgb="FF232629"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,12 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +502,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,16 +514,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -529,13 +531,13 @@
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -543,13 +545,13 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -557,13 +559,13 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -571,7 +573,7 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -585,7 +587,7 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -596,44 +598,44 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated and added employment by industry
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68B2975-8CBE-47B6-AEB1-A62A855B0290}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9735BD66-8C64-4C93-8643-31D732038AB9}"/>
   <bookViews>
     <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Data​</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>February 2023</t>
+  </si>
+  <si>
+    <t>Employment by industry</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,6 +648,20 @@
         <v>30</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add latest ilr data update data table
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68B2975-8CBE-47B6-AEB1-A62A855B0290}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B7011AE-B81D-4CD5-A5B0-5B8CBE1058CB}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Data​</t>
   </si>
@@ -80,24 +80,9 @@
     <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS online job adverts&lt;/a&gt;</t>
   </si>
   <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/3960ad0f-fd8a-49bb-91d7-f3ca1181b93f'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Jan 2022 (25/05/22)</t>
   </si>
   <si>
-    <t>Aug 2020 – Jul 2021 (25/11/21)</t>
-  </si>
-  <si>
-    <t>Aug 2021 – Apr 2022 (provisional) (20/07/22)</t>
-  </si>
-  <si>
-    <t>Aug 2021 – Jul 2022 (Nov 22)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Enterprise by employment size</t>
   </si>
   <si>
@@ -129,6 +114,18 @@
   </si>
   <si>
     <t>February 2023</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2021 – Jul 2022 (24/11/22)</t>
+  </si>
+  <si>
+    <t>Aug 2022 – Jan 2023 (Mar 23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -507,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,7 +552,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -569,7 +566,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -580,13 +577,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -594,55 +591,55 @@
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ILR SSA data updated charts to incorporate the ,atest ILR year. added some text about the per 100,000 method
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="262" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B7011AE-B81D-4CD5-A5B0-5B8CBE1058CB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="3640" yWindow="3640" windowWidth="16920" windowHeight="10540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated and added enterprise tab
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B7011AE-B81D-4CD5-A5B0-5B8CBE1058CB}"/>
+  <xr:revisionPtr revIDLastSave="287" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55EBE2B-97E9-49AF-A05B-B801DE917A5D}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3640" windowWidth="16920" windowHeight="10540" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Data​</t>
   </si>
@@ -89,12 +89,6 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Count&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Oct 2021 - Sept 2022 (28/09/22)</t>
-  </si>
-  <si>
-    <t>Oct 2022 - Sept 2023 (03/10/23)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
   </si>
   <si>
@@ -126,6 +120,27 @@
   </si>
   <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mar 2022 (28/09/22)</t>
+  </si>
+  <si>
+    <t>Mar 2023 (03/10/23)</t>
+  </si>
+  <si>
+    <t>Employment by industry</t>
+  </si>
+  <si>
+    <t>Enterprise by employment size and industry</t>
+  </si>
+  <si>
+    <t>Qualification by age and gender - NVQ</t>
+  </si>
+  <si>
+    <t>Jan 2021 - Dec 2021 (20/04/21)</t>
+  </si>
+  <si>
+    <t>Jan 2022 - Dec 2022 (19/04/22)</t>
   </si>
 </sst>
 </file>
@@ -502,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A12" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,7 +528,7 @@
     <col min="1" max="1" width="53.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="174.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
@@ -552,94 +567,136 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>19</v>
+      <c r="A8" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>25</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned, added and updated dashboard
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="287" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55EBE2B-97E9-49AF-A05B-B801DE917A5D}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{696D7C5E-E134-493E-B4D5-14E3C0852976}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Data​</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Enterprise by employment size</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Count&lt;/a&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
   </si>
   <si>
@@ -141,6 +138,21 @@
   </si>
   <si>
     <t>Jan 2022 - Dec 2022 (19/04/22)</t>
+  </si>
+  <si>
+    <t>Business demography</t>
+  </si>
+  <si>
+    <t>&lt;a href=' https://www.ons.gov.uk/businessindustryandtrade/business/activitysizeandlocation/datasets/businessdemographyreferencetable'&gt;ONS Business Demography&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Counts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>2022 (16/11/23)</t>
+  </si>
+  <si>
+    <t>2021 (17/11/22)</t>
   </si>
 </sst>
 </file>
@@ -517,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A12" sqref="A2:A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -575,7 +587,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -606,13 +618,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -620,27 +632,27 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -648,55 +660,69 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
+      <c r="A11" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>23</v>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sections for overview page
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="303" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{696D7C5E-E134-493E-B4D5-14E3C0852976}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added in various changes
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{696D7C5E-E134-493E-B4D5-14E3C0852976}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE98BC5F-1261-4CB5-96ED-0ED6BA241AE7}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Jan 2022 (25/05/22)</t>
   </si>
   <si>
-    <t>Enterprise by employment size</t>
-  </si>
-  <si>
     <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
   </si>
   <si>
@@ -128,12 +125,6 @@
     <t>Employment by industry</t>
   </si>
   <si>
-    <t>Enterprise by employment size and industry</t>
-  </si>
-  <si>
-    <t>Qualification by age and gender - NVQ</t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (20/04/21)</t>
   </si>
   <si>
@@ -153,6 +144,15 @@
   </si>
   <si>
     <t>2021 (17/11/22)</t>
+  </si>
+  <si>
+    <t>Highest qualification level by age and gender</t>
+  </si>
+  <si>
+    <t>Enterprises by employment size band</t>
+  </si>
+  <si>
+    <t>Enterprises by employment size band and industry</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -618,13 +618,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -632,97 +632,97 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data table text change
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="311" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01BDDD7A-DB6F-4CE2-9F2C-F42E868FD9FC}"/>
+  <xr:revisionPtr revIDLastSave="317" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2E7CD01-2264-4EBC-A702-42FABD45BBD2}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,12 +83,6 @@
     <t>Jan 2022 (25/05/22)</t>
   </si>
   <si>
-    <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key Stage 5 (KS5) destinations </t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/75e2be32-3c51-4790-2c28-08dab0fa305d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>February 2023</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -153,6 +144,15 @@
   </si>
   <si>
     <t>Dec 2021 - Dec 2022 (16/11/23)</t>
+  </si>
+  <si>
+    <t>Key Stage 4 (KS4) destinations  - provisional</t>
+  </si>
+  <si>
+    <t>Key Stage 5 (KS5) destinations - provisional</t>
+  </si>
+  <si>
+    <t>February 2023 - revision</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -618,13 +618,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -632,97 +632,97 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added downloads to the table reomved vacancy tab
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2E7CD01-2264-4EBC-A702-42FABD45BBD2}"/>
+  <xr:revisionPtr revIDLastSave="323" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C620C6-087A-4904-A7FE-F9EDD73C2A36}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -68,21 +68,12 @@
     <t>Employment share by occupation</t>
   </si>
   <si>
-    <t>Online job adverts by local authority</t>
-  </si>
-  <si>
     <t>Further education and skills achievements</t>
   </si>
   <si>
     <t>Further education and skills achievements by sector subject area</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS online job adverts&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Jan 2022 (25/05/22)</t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
@@ -153,13 +144,22 @@
   </si>
   <si>
     <t>February 2023 - revision</t>
+  </si>
+  <si>
+    <t>Job adverts by profession</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityuk'&gt;ONS Textkernel&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Oct 2022 (21/12/22)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +187,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF323132"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,13 +214,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -531,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -587,7 +594,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -599,21 +606,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -621,108 +628,108 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>27</v>
+      <c r="A11" t="s">
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>38</v>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updtae data update data table update text
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/ali_othman_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sula_marshall_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{0C6CFC05-59B6-4CCC-ACF4-4BE56BB7741B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A68B2975-8CBE-47B6-AEB1-A62A855B0290}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD775DDB-EC22-4024-BDB2-66F03C719AA8}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Data​</t>
   </si>
@@ -53,9 +53,6 @@
     <t>&lt;a href='https://www.nomisweb.co.uk/datasets/apsnew'&gt;Annual Population Survey&lt;/a&gt;</t>
   </si>
   <si>
-    <t>Jul 2021 - Jun 2022 (11/10/22)</t>
-  </si>
-  <si>
     <t>Oct 2021 - Sep 2022 (17/01/23)</t>
   </si>
   <si>
@@ -68,74 +65,98 @@
     <t>Employment share by occupation</t>
   </si>
   <si>
-    <t>Online job adverts by local authority</t>
-  </si>
-  <si>
     <t>Further education and skills achievements</t>
   </si>
   <si>
     <t>Further education and skills achievements by sector subject area</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/onlinejobadvertsbyitl1regionandlocalauthority'&gt;ONS online job adverts&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/3960ad0f-fd8a-49bb-91d7-f3ca1181b93f'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Jan 2022 (25/05/22)</t>
-  </si>
-  <si>
-    <t>Aug 2020 – Jul 2021 (25/11/21)</t>
-  </si>
-  <si>
-    <t>Aug 2021 – Apr 2022 (provisional) (20/07/22)</t>
-  </si>
-  <si>
-    <t>Aug 2021 – Jul 2022 (Nov 22)</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/61db0688-4ec0-4cfe-9e83-24d4ea9d078e'&gt;Individualised Learner Record&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Enterprise by employment size</t>
-  </si>
-  <si>
-    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Count&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Oct 2021 - Sept 2022 (28/09/22)</t>
-  </si>
-  <si>
-    <t>Oct 2022 - Sept 2023 (03/10/23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key Stage 4 (KS4) destinations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key Stage 5 (KS5) destinations </t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
-    <t>Aug 2020 -  Jul 2021 (2020 leavers) (20/10/22)</t>
-  </si>
-  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/62b04091-a13b-40e9-52d9-08dab0fd4449'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/75e2be32-3c51-4790-2c28-08dab0fa305d'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
-    <t>February 2023</t>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2021 – Jul 2022 (24/11/22)</t>
+  </si>
+  <si>
+    <t>Aug 2022 – Jan 2023 (Mar 23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-tables/permalink/cae2bcbb-e385-4da7-8d7b-08dacbbccc68'&gt;Individualised Learner Record&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Mar 2022 (28/09/22)</t>
+  </si>
+  <si>
+    <t>Mar 2023 (03/10/23)</t>
+  </si>
+  <si>
+    <t>Employment by industry</t>
+  </si>
+  <si>
+    <t>Business demography</t>
+  </si>
+  <si>
+    <t>&lt;a href=' https://www.ons.gov.uk/businessindustryandtrade/business/activitysizeandlocation/datasets/businessdemographyreferencetable'&gt;ONS Business Demography&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.nomisweb.co.uk/datasets/idbrent'&gt;ONS UK Business Counts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Highest qualification level by age and gender</t>
+  </si>
+  <si>
+    <t>Enterprises by employment size band</t>
+  </si>
+  <si>
+    <t>Enterprises by employment size band and industry</t>
+  </si>
+  <si>
+    <t>Aug 2020 -  Jul 2021 (19/20 learners) (20/10/22)</t>
+  </si>
+  <si>
+    <t>Dec 2020 - Dec 2021 (17/11/22)</t>
+  </si>
+  <si>
+    <t>Dec 2021 - Dec 2022 (16/11/23)</t>
+  </si>
+  <si>
+    <t>Key Stage 4 (KS4) destinations  - provisional</t>
+  </si>
+  <si>
+    <t>Key Stage 5 (KS5) destinations - provisional</t>
+  </si>
+  <si>
+    <t>February 2023 - revision</t>
+  </si>
+  <si>
+    <t>Job adverts by profession</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityuk'&gt;ONS Textkernel&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Oct 2022 (21/12/22)</t>
+  </si>
+  <si>
+    <t>Jan 2021 - Dec 2021 (20/04/22)</t>
+  </si>
+  <si>
+    <t>Jan 2022 - Dec 2022 (19/04/23)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +184,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF323132"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,13 +211,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,21 +534,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="53.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="174.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="174.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="41.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,116 +561,172 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="125.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loaded in new destinations data crrected small mistake in ilr data tidy code
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sula_marshall_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD775DDB-EC22-4024-BDB2-66F03C719AA8}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C513B01F-0CD0-4B29-9238-B17105868D67}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,12 +74,6 @@
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/62b04091-a13b-40e9-52d9-08dab0fd4449'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/75e2be32-3c51-4790-2c28-08dab0fa305d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -128,12 +122,6 @@
     <t>Dec 2021 - Dec 2022 (16/11/23)</t>
   </si>
   <si>
-    <t>Key Stage 4 (KS4) destinations  - provisional</t>
-  </si>
-  <si>
-    <t>Key Stage 5 (KS5) destinations - provisional</t>
-  </si>
-  <si>
     <t>February 2023 - revision</t>
   </si>
   <si>
@@ -150,6 +138,18 @@
   </si>
   <si>
     <t>Jan 2022 - Dec 2022 (19/04/23)</t>
+  </si>
+  <si>
+    <t>Key Stage 4 (KS4) destinations</t>
+  </si>
+  <si>
+    <t>Key Stage 5 (KS5) destinations</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1683bef5-5daa-49d7-9323-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,17 +537,17 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="174.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="174.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -572,10 +572,10 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="125.05" customHeight="1" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -586,12 +586,12 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -600,130 +600,130 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="C13" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
update veriosn control update data table
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C513B01F-0CD0-4B29-9238-B17105868D67}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B1D9746-1A54-45E5-AFDB-F429212509A7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -113,18 +113,12 @@
     <t>Enterprises by employment size band and industry</t>
   </si>
   <si>
-    <t>Aug 2020 -  Jul 2021 (19/20 learners) (20/10/22)</t>
-  </si>
-  <si>
     <t>Dec 2020 - Dec 2021 (17/11/22)</t>
   </si>
   <si>
     <t>Dec 2021 - Dec 2022 (16/11/23)</t>
   </si>
   <si>
-    <t>February 2023 - revision</t>
-  </si>
-  <si>
     <t>Job adverts by profession</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2020 -  Jul 2021 (19/20 learners) (02/02/23)</t>
+  </si>
+  <si>
+    <t>Aug 2021 -  Jul 2022 (20/21 learners) (Oct 23)</t>
   </si>
 </sst>
 </file>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="D12" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +572,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
@@ -586,7 +586,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -600,7 +600,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -639,10 +639,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -681,49 +681,49 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
update destinations data fix a few library issues
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/sula_marshall_education_gov_uk/Documents/Documents/lsip_dashboard/Data/8_DataTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD775DDB-EC22-4024-BDB2-66F03C719AA8}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3498B417-3B19-44C8-BE74-7A55A8F0697C}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12497" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,12 +74,6 @@
     <t>Jan 2021 - Dec 2021 (12/04/22)</t>
   </si>
   <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/62b04091-a13b-40e9-52d9-08dab0fd4449'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/75e2be32-3c51-4790-2c28-08dab0fa305d'&gt;National Pupil Database&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>&lt;a href='https://explore-education-statistics.service.gov.uk/data-catalogue/further-education-and-skills/2021-22'&gt;Individualised Learner Record&lt;/a&gt;</t>
   </si>
   <si>
@@ -119,24 +113,12 @@
     <t>Enterprises by employment size band and industry</t>
   </si>
   <si>
-    <t>Aug 2020 -  Jul 2021 (19/20 learners) (20/10/22)</t>
-  </si>
-  <si>
     <t>Dec 2020 - Dec 2021 (17/11/22)</t>
   </si>
   <si>
     <t>Dec 2021 - Dec 2022 (16/11/23)</t>
   </si>
   <si>
-    <t>Key Stage 4 (KS4) destinations  - provisional</t>
-  </si>
-  <si>
-    <t>Key Stage 5 (KS5) destinations - provisional</t>
-  </si>
-  <si>
-    <t>February 2023 - revision</t>
-  </si>
-  <si>
     <t>Job adverts by profession</t>
   </si>
   <si>
@@ -150,6 +132,24 @@
   </si>
   <si>
     <t>Jan 2022 - Dec 2022 (19/04/23)</t>
+  </si>
+  <si>
+    <t>Key Stage 4 (KS4) destinations</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1683bef5-5daa-49d7-9323-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>Aug 2020 -  Jul 2021 (19/20 learners) (02/02/23)</t>
+  </si>
+  <si>
+    <t>Aug 2021 -  Jul 2022 (20/21 learners) (Oct 23)</t>
+  </si>
+  <si>
+    <t>Key Stage 5 (KS5) destinations</t>
+  </si>
+  <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -211,15 +211,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +525,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -534,200 +533,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="174.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="174.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="41.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="125.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
add in new ons data
</commit_message>
<xml_diff>
--- a/Data/8_DataTable/221004DataTable.xlsx
+++ b/Data/8_DataTable/221004DataTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/8_DataTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3498B417-3B19-44C8-BE74-7A55A8F0697C}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{29948A3F-D1B6-493F-8855-7BED4738A843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FECAB5A-EC5F-481D-A6BE-476035A42986}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{677CE7B9-0003-4845-87B7-4FABD7ACD82F}"/>
   </bookViews>
@@ -122,12 +122,6 @@
     <t>Job adverts by profession</t>
   </si>
   <si>
-    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityuk'&gt;ONS Textkernel&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>Oct 2022 (21/12/22)</t>
-  </si>
-  <si>
     <t>Jan 2021 - Dec 2021 (20/04/22)</t>
   </si>
   <si>
@@ -137,19 +131,25 @@
     <t>Key Stage 4 (KS4) destinations</t>
   </si>
   <si>
+    <t>Key Stage 5 (KS5) destinations</t>
+  </si>
+  <si>
     <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1683bef5-5daa-49d7-9323-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
   </si>
   <si>
+    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
+  </si>
+  <si>
     <t>Aug 2020 -  Jul 2021 (19/20 learners) (02/02/23)</t>
   </si>
   <si>
     <t>Aug 2021 -  Jul 2022 (20/21 learners) (Oct 23)</t>
   </si>
   <si>
-    <t>Key Stage 5 (KS5) destinations</t>
-  </si>
-  <si>
-    <t>&lt;a href = 'https://explore-education-statistics.service.gov.uk/data-tables/permalink/1703fe2c-2e57-4bfe-9325-08db08498a11'&gt;National Pupil Database&lt;/a&gt;</t>
+    <t>Dec 2022 (13/02/23)</t>
+  </si>
+  <si>
+    <t>&lt;a href='https://www.ons.gov.uk/employmentandlabourmarket/peopleinwork/employmentandemployeetypes/datasets/labourdemandvolumesbyprofessionandlocalauthorityukjanuary2017todecember2022'&gt;ONS Textkernel&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -211,14 +211,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6050695-7AD5-4EAF-ACCC-796FB129457A}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,67 +547,63 @@
     <col min="3" max="3" width="27.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="125" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -616,12 +613,11 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:4" ht="83.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -631,115 +627,107 @@
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>